<commit_message>
Got Athens data working
</commit_message>
<xml_diff>
--- a/working/KreutzPFAS/UC_276_467_Athens_Mix 2a and b20220913.xlsx
+++ b/working/KreutzPFAS/UC_276_467_Athens_Mix 2a and b20220913.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\PRIV\CCTE_Wetmore-Lab\_PFAS_TK\PFAS_Analytical\GCMS\Reports\from Athens\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\invitrotkstats\working\KreutzPFAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C3DB91-0F96-490C-AD54-CCDB04B9A5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9244DE-55B2-469D-BD93-99DD199A133C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1_Mix 2a and b" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>Mix 2 CC 6</t>
   </si>
@@ -156,15 +156,6 @@
     <t>nm after crash</t>
   </si>
   <si>
-    <t>Mix 2a and b UCF sample data from Jens experiment</t>
-  </si>
-  <si>
-    <t>Multiple data points represent ANALYTICAL replicates (injected n=2 on instrument from one aliquot)</t>
-  </si>
-  <si>
-    <t>Standard check (cc) samples ran throughtout analysis for QAQC concentration checks</t>
-  </si>
-  <si>
     <t>split peak, REDO, but included in analysis</t>
   </si>
   <si>
@@ -190,7 +181,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,13 +192,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -257,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -273,14 +257,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -423,7 +403,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$A$6:$A$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$A$5:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -477,7 +457,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$D$6:$D$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$D$5:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -574,7 +554,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$A$6:$A$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$A$5:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -628,7 +608,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$F$6:$F$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$F$5:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -725,7 +705,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$A$6:$A$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$A$5:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -779,7 +759,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$G$6:$G$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$G$5:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -876,7 +856,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$A$6:$A$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$A$5:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -930,7 +910,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$I$6:$I$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$I$5:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1027,7 +1007,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$A$6:$A$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$A$5:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1081,7 +1061,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$J$6:$J$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$J$5:$J$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1526,7 +1506,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$A$6:$A$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$A$5:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1580,7 +1560,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$L$6:$L$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$L$5:$L$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1727,7 +1707,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$A$6:$A$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$A$5:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1781,7 +1761,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$M$6:$M$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$M$5:$M$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1928,7 +1908,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$A$6:$A$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$A$5:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1982,7 +1962,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$N$6:$N$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$N$5:$N$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2129,7 +2109,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$A$6:$A$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$A$5:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2183,7 +2163,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$O$6:$O$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$O$5:$O$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2330,7 +2310,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$A$6:$A$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$A$5:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2384,7 +2364,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1_Mix 2a and b'!$P$6:$P$20</c:f>
+              <c:f>'Sheet 1_Mix 2a and b'!$P$5:$P$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3779,13 +3759,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3815,14 +3795,14 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3853,14 +3833,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>562221</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>179172</xdr:rowOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>163297</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3897,13 +3877,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>539996</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>1372</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3941,13 +3921,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>25646</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>112243</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4305,10 +4285,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4316,9 +4296,9 @@
     <col min="1" max="1" width="18.54296875" customWidth="1"/>
     <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1796875" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="9" customWidth="1"/>
     <col min="5" max="5" width="9.1796875" customWidth="1"/>
-    <col min="6" max="7" width="9.1796875" style="10" customWidth="1"/>
+    <col min="6" max="7" width="9.1796875" style="9" customWidth="1"/>
     <col min="8" max="8" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4329,16 +4309,16 @@
       <c r="C1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="10">
+      <c r="D1" s="9">
         <v>471</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="10">
+      <c r="F1" s="9">
         <v>478</v>
       </c>
-      <c r="G1" s="10">
+      <c r="G1" s="9">
         <v>468</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -4355,16 +4335,16 @@
       <c r="C2" s="4">
         <v>269</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>187</v>
       </c>
       <c r="E2" s="4">
         <v>369</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>319</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="9">
         <v>321</v>
       </c>
       <c r="H2" s="4">
@@ -4384,16 +4364,16 @@
       <c r="C3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>39</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -4409,22 +4389,25 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
       <c r="B4" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="4">
         <v>6</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>6.8</v>
       </c>
       <c r="E4" s="4">
         <v>8.4</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>9.6999999999999993</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>9.6999999999999993</v>
       </c>
       <c r="H4" s="4">
@@ -4436,1530 +4419,1428 @@
       <c r="J4" s="6">
         <v>13.5</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5">
+        <v>0.17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>18865</v>
+      </c>
+      <c r="D5" s="9">
+        <v>142</v>
+      </c>
+      <c r="E5" s="4">
+        <v>17782</v>
+      </c>
+      <c r="F5" s="9">
+        <v>180</v>
+      </c>
+      <c r="G5" s="9">
         <v>40</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="L5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>49</v>
+      <c r="H5" s="4">
+        <v>13607</v>
+      </c>
+      <c r="I5" s="6">
+        <v>252</v>
+      </c>
+      <c r="J5" s="6">
+        <v>63</v>
+      </c>
+      <c r="L5" s="5">
+        <f>D5/E5</f>
+        <v>7.9856034191879421E-3</v>
+      </c>
+      <c r="M5" s="5">
+        <f>F5/E5</f>
+        <v>1.0122595883477675E-2</v>
+      </c>
+      <c r="N5" s="6">
+        <f>G5/E5</f>
+        <v>2.2494657518839275E-3</v>
+      </c>
+      <c r="O5" s="6">
+        <f>I5/E5</f>
+        <v>1.4171634236868744E-2</v>
+      </c>
+      <c r="P5" s="6">
+        <f>J5/E5</f>
+        <v>3.542908559217186E-3</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>0.17</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4">
-        <v>18865</v>
-      </c>
-      <c r="D6" s="10">
-        <v>142</v>
+        <v>18290</v>
+      </c>
+      <c r="D6" s="9">
+        <v>314</v>
       </c>
       <c r="E6" s="4">
-        <v>17782</v>
-      </c>
-      <c r="F6" s="10">
-        <v>180</v>
-      </c>
-      <c r="G6" s="10">
-        <v>40</v>
+        <v>16512</v>
+      </c>
+      <c r="F6" s="9">
+        <v>214</v>
+      </c>
+      <c r="G6" s="9">
+        <v>146</v>
       </c>
       <c r="H6" s="4">
-        <v>13607</v>
+        <v>6530</v>
       </c>
       <c r="I6" s="6">
-        <v>252</v>
+        <v>342</v>
       </c>
       <c r="J6" s="6">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="L6" s="5">
-        <f>D6/E6</f>
-        <v>7.9856034191879421E-3</v>
+        <f t="shared" ref="L6:L19" si="0">D6/E6</f>
+        <v>1.9016472868217053E-2</v>
       </c>
       <c r="M6" s="5">
-        <f>F6/E6</f>
-        <v>1.0122595883477675E-2</v>
+        <f t="shared" ref="M6:M19" si="1">F6/E6</f>
+        <v>1.2960271317829458E-2</v>
       </c>
       <c r="N6" s="6">
-        <f>G6/E6</f>
-        <v>2.2494657518839275E-3</v>
+        <f t="shared" ref="N6:N19" si="2">G6/E6</f>
+        <v>8.8420542635658916E-3</v>
       </c>
       <c r="O6" s="6">
-        <f>I6/E6</f>
-        <v>1.4171634236868744E-2</v>
+        <f t="shared" ref="O6:O19" si="3">I6/E6</f>
+        <v>2.071220930232558E-2</v>
       </c>
       <c r="P6" s="6">
-        <f>J6/E6</f>
-        <v>3.542908559217186E-3</v>
+        <f t="shared" ref="P6:P19" si="4">J6/E6</f>
+        <v>6.1773255813953485E-3</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>0.28000000000000003</v>
+        <v>0.44</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4">
-        <v>18290</v>
-      </c>
-      <c r="D7" s="10">
-        <v>314</v>
+        <v>17767</v>
+      </c>
+      <c r="D7" s="9">
+        <v>786</v>
       </c>
       <c r="E7" s="4">
-        <v>16512</v>
-      </c>
-      <c r="F7" s="10">
-        <v>214</v>
-      </c>
-      <c r="G7" s="10">
-        <v>146</v>
+        <v>19577</v>
+      </c>
+      <c r="F7" s="9">
+        <v>486</v>
+      </c>
+      <c r="G7" s="9">
+        <v>113</v>
       </c>
       <c r="H7" s="4">
-        <v>6530</v>
+        <v>7369</v>
       </c>
       <c r="I7" s="6">
-        <v>342</v>
+        <v>580</v>
       </c>
       <c r="J7" s="6">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="L7" s="5">
-        <f t="shared" ref="L7:L20" si="0">D7/E7</f>
-        <v>1.9016472868217053E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.0149154620217599E-2</v>
       </c>
       <c r="M7" s="5">
-        <f t="shared" ref="M7:M20" si="1">F7/E7</f>
-        <v>1.2960271317829458E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.4825049803340656E-2</v>
       </c>
       <c r="N7" s="6">
-        <f t="shared" ref="N7:N20" si="2">G7/E7</f>
-        <v>8.8420542635658916E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.77207948102365E-3</v>
       </c>
       <c r="O7" s="6">
-        <f t="shared" ref="O7:O20" si="3">I7/E7</f>
-        <v>2.071220930232558E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.9626602645962098E-2</v>
       </c>
       <c r="P7" s="6">
-        <f t="shared" ref="P7:P20" si="4">J7/E7</f>
-        <v>6.1773255813953485E-3</v>
+        <f t="shared" si="4"/>
+        <v>7.2023292639321656E-3</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>0.44</v>
+        <v>0.71</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C8" s="4">
-        <v>17767</v>
-      </c>
-      <c r="D8" s="10">
-        <v>786</v>
+        <v>18188</v>
+      </c>
+      <c r="D8" s="9">
+        <v>228</v>
       </c>
       <c r="E8" s="4">
-        <v>19577</v>
-      </c>
-      <c r="F8" s="10">
-        <v>486</v>
-      </c>
-      <c r="G8" s="10">
-        <v>113</v>
+        <v>18369</v>
+      </c>
+      <c r="F8" s="9">
+        <v>582</v>
+      </c>
+      <c r="G8" s="9">
+        <v>97</v>
       </c>
       <c r="H8" s="4">
-        <v>7369</v>
+        <v>8634</v>
       </c>
       <c r="I8" s="6">
-        <v>580</v>
+        <v>638</v>
       </c>
       <c r="J8" s="6">
-        <v>141</v>
+        <v>219</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="0"/>
-        <v>4.0149154620217599E-2</v>
+        <v>1.2412216233872285E-2</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="1"/>
-        <v>2.4825049803340656E-2</v>
+        <v>3.1683815123305571E-2</v>
       </c>
       <c r="N8" s="6">
         <f t="shared" si="2"/>
-        <v>5.77207948102365E-3</v>
+        <v>5.2806358538842616E-3</v>
       </c>
       <c r="O8" s="6">
         <f t="shared" si="3"/>
-        <v>2.9626602645962098E-2</v>
+        <v>3.4732429636888239E-2</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" si="4"/>
-        <v>7.2023292639321656E-3</v>
+        <v>1.1922260329903641E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>0.71</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4">
-        <v>18188</v>
-      </c>
-      <c r="D9" s="10">
-        <v>228</v>
+        <v>19565</v>
+      </c>
+      <c r="D9" s="9">
+        <v>567</v>
       </c>
       <c r="E9" s="4">
-        <v>18369</v>
-      </c>
-      <c r="F9" s="10">
-        <v>582</v>
-      </c>
-      <c r="G9" s="10">
-        <v>97</v>
+        <v>16111</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1294</v>
+      </c>
+      <c r="G9" s="9">
+        <v>115</v>
       </c>
       <c r="H9" s="4">
-        <v>8634</v>
+        <v>7246</v>
       </c>
       <c r="I9" s="6">
-        <v>638</v>
+        <v>1368</v>
       </c>
       <c r="J9" s="6">
-        <v>219</v>
+        <v>291</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="0"/>
-        <v>1.2412216233872285E-2</v>
+        <v>3.5193346161008006E-2</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="1"/>
-        <v>3.1683815123305571E-2</v>
+        <v>8.0317795295139965E-2</v>
       </c>
       <c r="N9" s="6">
         <f t="shared" si="2"/>
-        <v>5.2806358538842616E-3</v>
+        <v>7.1379802619328412E-3</v>
       </c>
       <c r="O9" s="6">
         <f t="shared" si="3"/>
-        <v>3.4732429636888239E-2</v>
+        <v>8.4910930420209793E-2</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="4"/>
-        <v>1.1922260329903641E-2</v>
+        <v>1.8062193532369188E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>1.1399999999999999</v>
+        <v>1.82</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C10" s="4">
-        <v>19565</v>
-      </c>
-      <c r="D10" s="10">
-        <v>567</v>
+        <v>21802</v>
+      </c>
+      <c r="D10" s="9">
+        <v>534</v>
       </c>
       <c r="E10" s="4">
-        <v>16111</v>
-      </c>
-      <c r="F10" s="10">
-        <v>1294</v>
-      </c>
-      <c r="G10" s="10">
-        <v>115</v>
+        <v>17100</v>
+      </c>
+      <c r="F10" s="9">
+        <v>1225</v>
+      </c>
+      <c r="G10" s="9">
+        <v>116</v>
       </c>
       <c r="H10" s="4">
-        <v>7246</v>
-      </c>
-      <c r="I10" s="6">
-        <v>1368</v>
-      </c>
-      <c r="J10" s="6">
-        <v>291</v>
+        <v>15985</v>
+      </c>
+      <c r="I10" s="8">
+        <v>2037</v>
+      </c>
+      <c r="J10" s="8">
+        <v>451</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="0"/>
-        <v>3.5193346161008006E-2</v>
+        <v>3.1228070175438598E-2</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="1"/>
-        <v>8.0317795295139965E-2</v>
+        <v>7.1637426900584791E-2</v>
       </c>
       <c r="N10" s="6">
         <f t="shared" si="2"/>
-        <v>7.1379802619328412E-3</v>
+        <v>6.7836257309941521E-3</v>
       </c>
       <c r="O10" s="6">
         <f t="shared" si="3"/>
-        <v>8.4910930420209793E-2</v>
+        <v>0.11912280701754387</v>
       </c>
       <c r="P10" s="6">
         <f t="shared" si="4"/>
-        <v>1.8062193532369188E-2</v>
+        <v>2.6374269005847953E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>1.82</v>
+        <v>2.91</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C11" s="4">
-        <v>21802</v>
-      </c>
-      <c r="D11" s="10">
-        <v>534</v>
+        <v>18946</v>
+      </c>
+      <c r="D11" s="9">
+        <v>887</v>
       </c>
       <c r="E11" s="4">
-        <v>17100</v>
-      </c>
-      <c r="F11" s="10">
-        <v>1225</v>
-      </c>
-      <c r="G11" s="10">
-        <v>116</v>
+        <v>15407</v>
+      </c>
+      <c r="F11" s="9">
+        <v>2414</v>
+      </c>
+      <c r="G11" s="9">
+        <v>70</v>
       </c>
       <c r="H11" s="4">
-        <v>15985</v>
-      </c>
-      <c r="I11" s="8">
-        <v>2037</v>
-      </c>
-      <c r="J11" s="8">
-        <v>451</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>44</v>
+        <v>9441</v>
+      </c>
+      <c r="I11" s="6">
+        <v>3039</v>
+      </c>
+      <c r="J11" s="6">
+        <v>465</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="0"/>
-        <v>3.1228070175438598E-2</v>
+        <v>5.7571233854741354E-2</v>
       </c>
       <c r="M11" s="5">
         <f t="shared" si="1"/>
-        <v>7.1637426900584791E-2</v>
+        <v>0.15668202764976957</v>
       </c>
       <c r="N11" s="6">
         <f t="shared" si="2"/>
-        <v>6.7836257309941521E-3</v>
+        <v>4.5433893684688779E-3</v>
       </c>
       <c r="O11" s="6">
         <f t="shared" si="3"/>
-        <v>0.11912280701754387</v>
+        <v>0.19724800415395599</v>
       </c>
       <c r="P11" s="6">
         <f t="shared" si="4"/>
-        <v>2.6374269005847953E-2</v>
+        <v>3.0181086519114688E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>2.91</v>
+        <v>4.66</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C12" s="4">
-        <v>18946</v>
-      </c>
-      <c r="D12" s="10">
-        <v>887</v>
+        <v>17705</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1545</v>
       </c>
       <c r="E12" s="4">
-        <v>15407</v>
-      </c>
-      <c r="F12" s="10">
-        <v>2414</v>
-      </c>
-      <c r="G12" s="10">
-        <v>70</v>
+        <v>16935</v>
+      </c>
+      <c r="F12" s="9">
+        <v>4636</v>
+      </c>
+      <c r="G12" s="9">
+        <v>82</v>
       </c>
       <c r="H12" s="4">
-        <v>9441</v>
+        <v>8008</v>
       </c>
       <c r="I12" s="6">
-        <v>3039</v>
+        <v>5047</v>
       </c>
       <c r="J12" s="6">
-        <v>465</v>
+        <v>793</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" si="0"/>
-        <v>5.7571233854741354E-2</v>
+        <v>9.12311780336581E-2</v>
       </c>
       <c r="M12" s="5">
         <f t="shared" si="1"/>
-        <v>0.15668202764976957</v>
+        <v>0.27375258340714498</v>
       </c>
       <c r="N12" s="6">
         <f t="shared" si="2"/>
-        <v>4.5433893684688779E-3</v>
+        <v>4.8420431059935046E-3</v>
       </c>
       <c r="O12" s="6">
         <f t="shared" si="3"/>
-        <v>0.19724800415395599</v>
+        <v>0.29802184824328315</v>
       </c>
       <c r="P12" s="6">
         <f t="shared" si="4"/>
-        <v>3.0181086519114688E-2</v>
+        <v>4.6826099793327428E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>4.66</v>
+        <v>7.45</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13" s="4">
-        <v>17705</v>
-      </c>
-      <c r="D13" s="10">
-        <v>1545</v>
+        <v>19809</v>
+      </c>
+      <c r="D13" s="9">
+        <v>2590</v>
       </c>
       <c r="E13" s="4">
-        <v>16935</v>
-      </c>
-      <c r="F13" s="10">
-        <v>4636</v>
-      </c>
-      <c r="G13" s="10">
-        <v>82</v>
+        <v>16340</v>
+      </c>
+      <c r="F13" s="9">
+        <v>8180</v>
+      </c>
+      <c r="G13" s="9">
+        <v>190</v>
       </c>
       <c r="H13" s="4">
-        <v>8008</v>
+        <v>6070</v>
       </c>
       <c r="I13" s="6">
-        <v>5047</v>
+        <v>8219</v>
       </c>
       <c r="J13" s="6">
-        <v>793</v>
+        <v>1111</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="0"/>
-        <v>9.12311780336581E-2</v>
+        <v>0.15850673194614442</v>
       </c>
       <c r="M13" s="5">
         <f t="shared" si="1"/>
-        <v>0.27375258340714498</v>
+        <v>0.5006119951040392</v>
       </c>
       <c r="N13" s="6">
         <f t="shared" si="2"/>
-        <v>4.8420431059935046E-3</v>
+        <v>1.1627906976744186E-2</v>
       </c>
       <c r="O13" s="6">
         <f t="shared" si="3"/>
-        <v>0.29802184824328315</v>
+        <v>0.50299877600979193</v>
       </c>
       <c r="P13" s="6">
         <f t="shared" si="4"/>
-        <v>4.6826099793327428E-2</v>
+        <v>6.799265605875153E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>7.45</v>
+        <v>11.92</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C14" s="4">
-        <v>19809</v>
-      </c>
-      <c r="D14" s="10">
-        <v>2590</v>
+        <v>17400</v>
+      </c>
+      <c r="D14" s="9">
+        <v>4242</v>
       </c>
       <c r="E14" s="4">
-        <v>16340</v>
-      </c>
-      <c r="F14" s="10">
-        <v>8180</v>
-      </c>
-      <c r="G14" s="10">
-        <v>190</v>
+        <v>15071</v>
+      </c>
+      <c r="F14" s="9">
+        <v>12774</v>
+      </c>
+      <c r="G14" s="9">
+        <v>149</v>
       </c>
       <c r="H14" s="4">
-        <v>6070</v>
+        <v>9673</v>
       </c>
       <c r="I14" s="6">
-        <v>8219</v>
+        <v>12356</v>
       </c>
       <c r="J14" s="6">
-        <v>1111</v>
+        <v>1957</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="0"/>
-        <v>0.15850673194614442</v>
+        <v>0.2814677194612169</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="1"/>
-        <v>0.5006119951040392</v>
+        <v>0.84758808307345235</v>
       </c>
       <c r="N14" s="6">
         <f t="shared" si="2"/>
-        <v>1.1627906976744186E-2</v>
+        <v>9.8865370579258177E-3</v>
       </c>
       <c r="O14" s="6">
         <f t="shared" si="3"/>
-        <v>0.50299877600979193</v>
+        <v>0.81985269723309673</v>
       </c>
       <c r="P14" s="6">
         <f t="shared" si="4"/>
-        <v>6.799265605875153E-2</v>
+        <v>0.12985203370711965</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>11.92</v>
+        <v>19.07</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" s="4">
-        <v>17400</v>
-      </c>
-      <c r="D15" s="10">
-        <v>4242</v>
+        <v>18828</v>
+      </c>
+      <c r="D15" s="9">
+        <v>6580</v>
       </c>
       <c r="E15" s="4">
-        <v>15071</v>
-      </c>
-      <c r="F15" s="10">
-        <v>12774</v>
-      </c>
-      <c r="G15" s="10">
-        <v>149</v>
+        <v>18616</v>
+      </c>
+      <c r="F15" s="9">
+        <v>19142</v>
+      </c>
+      <c r="G15" s="9">
+        <v>230</v>
       </c>
       <c r="H15" s="4">
-        <v>9673</v>
+        <v>17976</v>
       </c>
       <c r="I15" s="6">
-        <v>12356</v>
+        <v>18329</v>
       </c>
       <c r="J15" s="6">
-        <v>1957</v>
+        <v>2878</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="0"/>
-        <v>0.2814677194612169</v>
+        <v>0.35345938977223895</v>
       </c>
       <c r="M15" s="5">
         <f t="shared" si="1"/>
-        <v>0.84758808307345235</v>
+        <v>1.0282552642887839</v>
       </c>
       <c r="N15" s="6">
         <f t="shared" si="2"/>
-        <v>9.8865370579258177E-3</v>
+        <v>1.2354963472281908E-2</v>
       </c>
       <c r="O15" s="6">
         <f t="shared" si="3"/>
-        <v>0.81985269723309673</v>
+        <v>0.98458315427589171</v>
       </c>
       <c r="P15" s="6">
         <f t="shared" si="4"/>
-        <v>0.12985203370711965</v>
+        <v>0.15459819510098841</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>19.07</v>
+        <v>30.52</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C16" s="4">
-        <v>18828</v>
-      </c>
-      <c r="D16" s="10">
-        <v>6580</v>
+        <v>17967</v>
+      </c>
+      <c r="D16" s="9">
+        <v>14950</v>
       </c>
       <c r="E16" s="4">
-        <v>18616</v>
-      </c>
-      <c r="F16" s="10">
-        <v>19142</v>
-      </c>
-      <c r="G16" s="10">
-        <v>230</v>
+        <v>16164</v>
+      </c>
+      <c r="F16" s="9">
+        <v>44430</v>
+      </c>
+      <c r="G16" s="9">
+        <v>461</v>
       </c>
       <c r="H16" s="4">
-        <v>17976</v>
+        <v>7097</v>
       </c>
       <c r="I16" s="6">
-        <v>18329</v>
+        <v>36530</v>
       </c>
       <c r="J16" s="6">
-        <v>2878</v>
+        <v>5158</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="0"/>
-        <v>0.35345938977223895</v>
+        <v>0.92489482801286815</v>
       </c>
       <c r="M16" s="5">
         <f t="shared" si="1"/>
-        <v>1.0282552642887839</v>
+        <v>2.748700816629547</v>
       </c>
       <c r="N16" s="6">
         <f t="shared" si="2"/>
-        <v>1.2354963472281908E-2</v>
+        <v>2.8520168275179412E-2</v>
       </c>
       <c r="O16" s="6">
         <f t="shared" si="3"/>
-        <v>0.98458315427589171</v>
+        <v>2.2599604058401388</v>
       </c>
       <c r="P16" s="6">
         <f t="shared" si="4"/>
-        <v>0.15459819510098841</v>
+        <v>0.31910418213313535</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>30.52</v>
+        <v>48.83</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C17" s="4">
-        <v>17967</v>
-      </c>
-      <c r="D17" s="10">
-        <v>14950</v>
+        <v>19534</v>
+      </c>
+      <c r="D17" s="9">
+        <v>20649</v>
       </c>
       <c r="E17" s="4">
-        <v>16164</v>
-      </c>
-      <c r="F17" s="10">
-        <v>44430</v>
-      </c>
-      <c r="G17" s="10">
-        <v>461</v>
+        <v>14396</v>
+      </c>
+      <c r="F17" s="9">
+        <v>58965</v>
+      </c>
+      <c r="G17" s="9">
+        <v>513</v>
       </c>
       <c r="H17" s="4">
-        <v>7097</v>
+        <v>9416</v>
       </c>
       <c r="I17" s="6">
-        <v>36530</v>
+        <v>50548</v>
       </c>
       <c r="J17" s="6">
-        <v>5158</v>
+        <v>6740</v>
       </c>
       <c r="L17" s="5">
         <f t="shared" si="0"/>
-        <v>0.92489482801286815</v>
+        <v>1.434356765768269</v>
       </c>
       <c r="M17" s="5">
         <f t="shared" si="1"/>
-        <v>2.748700816629547</v>
+        <v>4.0959294248402331</v>
       </c>
       <c r="N17" s="6">
         <f t="shared" si="2"/>
-        <v>2.8520168275179412E-2</v>
+        <v>3.5634898582939709E-2</v>
       </c>
       <c r="O17" s="6">
         <f t="shared" si="3"/>
-        <v>2.2599604058401388</v>
+        <v>3.5112531258682966</v>
       </c>
       <c r="P17" s="6">
         <f t="shared" si="4"/>
-        <v>0.31910418213313535</v>
+        <v>0.46818560711308699</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>48.83</v>
+        <v>78.13</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C18" s="4">
-        <v>19534</v>
-      </c>
-      <c r="D18" s="10">
-        <v>20649</v>
+        <v>19590</v>
+      </c>
+      <c r="D18" s="9">
+        <v>32785</v>
       </c>
       <c r="E18" s="4">
-        <v>14396</v>
-      </c>
-      <c r="F18" s="10">
-        <v>58965</v>
-      </c>
-      <c r="G18" s="10">
-        <v>513</v>
+        <v>18463</v>
+      </c>
+      <c r="F18" s="9">
+        <v>91448</v>
+      </c>
+      <c r="G18" s="9">
+        <v>801</v>
       </c>
       <c r="H18" s="4">
-        <v>9416</v>
+        <v>17553</v>
       </c>
       <c r="I18" s="6">
-        <v>50548</v>
+        <v>81391</v>
       </c>
       <c r="J18" s="6">
-        <v>6740</v>
+        <v>11440</v>
       </c>
       <c r="L18" s="5">
         <f t="shared" si="0"/>
-        <v>1.434356765768269</v>
+        <v>1.7757135893408438</v>
       </c>
       <c r="M18" s="5">
         <f t="shared" si="1"/>
-        <v>4.0959294248402331</v>
+        <v>4.9530412175702754</v>
       </c>
       <c r="N18" s="6">
         <f t="shared" si="2"/>
-        <v>3.5634898582939709E-2</v>
+        <v>4.3384065428153602E-2</v>
       </c>
       <c r="O18" s="6">
         <f t="shared" si="3"/>
-        <v>3.5112531258682966</v>
+        <v>4.4083301738612359</v>
       </c>
       <c r="P18" s="6">
         <f t="shared" si="4"/>
-        <v>0.46818560711308699</v>
+        <v>0.61961761360558953</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>78.13</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C19" s="4">
-        <v>19590</v>
-      </c>
-      <c r="D19" s="10">
-        <v>32785</v>
+        <v>20584</v>
+      </c>
+      <c r="D19" s="9">
+        <v>65953</v>
       </c>
       <c r="E19" s="4">
-        <v>18463</v>
-      </c>
-      <c r="F19" s="10">
-        <v>91448</v>
-      </c>
-      <c r="G19" s="10">
-        <v>801</v>
+        <v>21740</v>
+      </c>
+      <c r="F19" s="9">
+        <v>193228</v>
+      </c>
+      <c r="G19" s="9">
+        <v>1714</v>
       </c>
       <c r="H19" s="4">
-        <v>17553</v>
+        <v>11984</v>
       </c>
       <c r="I19" s="6">
-        <v>81391</v>
+        <v>150399</v>
       </c>
       <c r="J19" s="6">
-        <v>11440</v>
+        <v>18845</v>
       </c>
       <c r="L19" s="5">
         <f t="shared" si="0"/>
-        <v>1.7757135893408438</v>
+        <v>3.0337166513339469</v>
       </c>
       <c r="M19" s="5">
         <f t="shared" si="1"/>
-        <v>4.9530412175702754</v>
+        <v>8.8881324747010115</v>
       </c>
       <c r="N19" s="6">
         <f t="shared" si="2"/>
-        <v>4.3384065428153602E-2</v>
+        <v>7.8840846366145356E-2</v>
       </c>
       <c r="O19" s="6">
         <f t="shared" si="3"/>
-        <v>4.4083301738612359</v>
+        <v>6.9180772769089236</v>
       </c>
       <c r="P19" s="6">
         <f t="shared" si="4"/>
-        <v>0.61961761360558953</v>
+        <v>0.86683532658693652</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>125</v>
-      </c>
       <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="4">
-        <v>20584</v>
-      </c>
-      <c r="D20" s="10">
-        <v>65953</v>
-      </c>
-      <c r="E20" s="4">
-        <v>21740</v>
-      </c>
-      <c r="F20" s="10">
-        <v>193228</v>
-      </c>
-      <c r="G20" s="10">
-        <v>1714</v>
-      </c>
-      <c r="H20" s="4">
-        <v>11984</v>
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="9">
+        <v>201</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="9">
+        <v>51</v>
+      </c>
+      <c r="G20" s="9">
+        <v>69</v>
+      </c>
+      <c r="H20" t="s">
+        <v>30</v>
       </c>
       <c r="I20" s="6">
-        <v>150399</v>
+        <v>35</v>
       </c>
       <c r="J20" s="6">
-        <v>18845</v>
-      </c>
-      <c r="L20" s="5">
-        <f t="shared" si="0"/>
-        <v>3.0337166513339469</v>
-      </c>
-      <c r="M20" s="5">
-        <f t="shared" si="1"/>
-        <v>8.8881324747010115</v>
-      </c>
-      <c r="N20" s="6">
-        <f t="shared" si="2"/>
-        <v>7.8840846366145356E-2</v>
-      </c>
-      <c r="O20" s="6">
-        <f t="shared" si="3"/>
-        <v>6.9180772769089236</v>
-      </c>
-      <c r="P20" s="6">
-        <f t="shared" si="4"/>
-        <v>0.86683532658693652</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="10">
-        <v>201</v>
-      </c>
-      <c r="E21" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="10">
-        <v>51</v>
-      </c>
-      <c r="G21" s="10">
-        <v>69</v>
-      </c>
-      <c r="H21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I21" s="6">
-        <v>35</v>
-      </c>
-      <c r="J21" s="6">
-        <v>26</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C21" s="4">
+        <v>21274</v>
+      </c>
+      <c r="D21" s="9">
+        <v>481</v>
+      </c>
+      <c r="E21" s="4">
+        <v>23284</v>
+      </c>
+      <c r="F21" s="9">
+        <v>255</v>
+      </c>
+      <c r="G21" s="12"/>
+      <c r="H21" s="4">
+        <v>10581</v>
+      </c>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="4">
+        <v>20285</v>
+      </c>
+      <c r="D22" s="9">
+        <v>291</v>
+      </c>
+      <c r="E22" s="4">
+        <v>25106</v>
+      </c>
+      <c r="F22" s="9">
+        <v>336</v>
+      </c>
+      <c r="G22" s="12"/>
+      <c r="H22" s="4">
+        <v>13386</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A23" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="4">
+        <v>20169</v>
+      </c>
+      <c r="D23" s="9">
+        <v>423</v>
+      </c>
+      <c r="E23" s="4">
+        <v>20310</v>
+      </c>
+      <c r="F23" s="9">
+        <v>274</v>
+      </c>
+      <c r="G23" s="12"/>
+      <c r="H23" s="4">
+        <v>11993</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="4">
+        <v>19612</v>
+      </c>
+      <c r="D24" s="9">
+        <v>210</v>
+      </c>
+      <c r="E24" s="4">
+        <v>23562</v>
+      </c>
+      <c r="F24" s="9">
+        <v>210</v>
+      </c>
+      <c r="G24" s="12"/>
+      <c r="H24" s="4">
+        <v>14089</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C25" s="4">
-        <v>21274</v>
-      </c>
-      <c r="D25" s="10">
-        <v>481</v>
+        <v>23013</v>
+      </c>
+      <c r="D25" s="9">
+        <v>334</v>
       </c>
       <c r="E25" s="4">
-        <v>23284</v>
-      </c>
-      <c r="F25" s="10">
-        <v>255</v>
-      </c>
-      <c r="G25" s="14"/>
+        <v>23811</v>
+      </c>
+      <c r="F25" s="9">
+        <v>184</v>
+      </c>
+      <c r="G25" s="12"/>
       <c r="H25" s="4">
-        <v>10581</v>
+        <v>8108</v>
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C26" s="4">
-        <v>20285</v>
-      </c>
-      <c r="D26" s="10">
-        <v>291</v>
+        <v>19622</v>
+      </c>
+      <c r="D26" s="9">
+        <v>131</v>
       </c>
       <c r="E26" s="4">
-        <v>25106</v>
-      </c>
-      <c r="F26" s="10">
-        <v>336</v>
-      </c>
-      <c r="G26" s="14"/>
+        <v>22627</v>
+      </c>
+      <c r="F26" s="9">
+        <v>157</v>
+      </c>
+      <c r="G26" s="12"/>
       <c r="H26" s="4">
-        <v>13386</v>
+        <v>13149</v>
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="C27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="4">
+        <v>21015</v>
+      </c>
+      <c r="E27" s="4">
+        <v>22503</v>
+      </c>
+      <c r="G27" s="9">
+        <v>20</v>
+      </c>
+      <c r="H27" s="4">
+        <v>7269</v>
+      </c>
+      <c r="I27" s="6">
+        <v>23888</v>
+      </c>
+      <c r="J27" s="6">
+        <v>4317</v>
+      </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C28" s="4">
-        <v>20169</v>
-      </c>
-      <c r="D28" s="10">
-        <v>423</v>
+        <v>20035</v>
       </c>
       <c r="E28" s="4">
-        <v>20310</v>
-      </c>
-      <c r="F28" s="10">
-        <v>274</v>
-      </c>
-      <c r="G28" s="14"/>
+        <v>21379</v>
+      </c>
+      <c r="G28" s="9">
+        <v>56</v>
+      </c>
       <c r="H28" s="4">
-        <v>11993</v>
-      </c>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+        <v>5610</v>
+      </c>
+      <c r="I28" s="6">
+        <v>21979</v>
+      </c>
+      <c r="J28" s="6">
+        <v>4592</v>
+      </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C29" s="4">
-        <v>19612</v>
-      </c>
-      <c r="D29" s="10">
-        <v>210</v>
+        <v>21318</v>
       </c>
       <c r="E29" s="4">
-        <v>23562</v>
-      </c>
-      <c r="F29" s="10">
-        <v>210</v>
-      </c>
-      <c r="G29" s="14"/>
+        <v>22962</v>
+      </c>
+      <c r="G29" s="9">
+        <v>51</v>
+      </c>
       <c r="H29" s="4">
-        <v>14089</v>
-      </c>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
+        <v>6649</v>
+      </c>
+      <c r="I29" s="6">
+        <v>10924</v>
+      </c>
+      <c r="J29" s="6">
+        <v>1984</v>
+      </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="C30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="4">
+        <v>18656</v>
+      </c>
+      <c r="E30" s="4">
+        <v>22022</v>
+      </c>
+      <c r="G30" s="9">
+        <v>66</v>
+      </c>
+      <c r="H30" s="4">
+        <v>6151</v>
+      </c>
+      <c r="I30" s="6">
+        <v>10280</v>
+      </c>
+      <c r="J30" s="6">
+        <v>2340</v>
+      </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C31" s="4">
-        <v>23013</v>
-      </c>
-      <c r="D31" s="10">
-        <v>334</v>
+        <v>21217</v>
       </c>
       <c r="E31" s="4">
-        <v>23811</v>
-      </c>
-      <c r="F31" s="10">
-        <v>184</v>
-      </c>
-      <c r="G31" s="14"/>
+        <v>22085</v>
+      </c>
+      <c r="G31" s="9">
+        <v>17</v>
+      </c>
       <c r="H31" s="4">
-        <v>8108</v>
-      </c>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+        <v>9374</v>
+      </c>
+      <c r="I31" s="6">
+        <v>17934</v>
+      </c>
+      <c r="J31" s="6">
+        <v>3190</v>
+      </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C32" s="4">
-        <v>19622</v>
-      </c>
-      <c r="D32" s="10">
-        <v>131</v>
+        <v>17999</v>
       </c>
       <c r="E32" s="4">
-        <v>22627</v>
-      </c>
-      <c r="F32" s="10">
-        <v>157</v>
-      </c>
-      <c r="G32" s="14"/>
+        <v>21987</v>
+      </c>
+      <c r="G32" s="9">
+        <v>74</v>
+      </c>
       <c r="H32" s="4">
-        <v>13149</v>
-      </c>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
+        <v>6044</v>
+      </c>
+      <c r="I32" s="6">
+        <v>16816</v>
+      </c>
+      <c r="J32" s="6">
+        <v>3571</v>
+      </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="H33" s="4"/>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="4">
+        <v>19278</v>
+      </c>
+      <c r="D33" s="9">
+        <v>593</v>
+      </c>
+      <c r="E33" s="4">
+        <v>20047</v>
+      </c>
+      <c r="F33" s="9">
+        <v>5142</v>
+      </c>
+      <c r="H33" s="4">
+        <v>7847</v>
+      </c>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="4">
+        <v>19311</v>
+      </c>
+      <c r="D34" s="9">
+        <v>559</v>
+      </c>
+      <c r="E34" s="4">
+        <v>20412</v>
+      </c>
+      <c r="F34" s="9">
+        <v>5383</v>
+      </c>
+      <c r="H34" s="4">
+        <v>6459</v>
+      </c>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="4">
+        <v>21519</v>
+      </c>
+      <c r="E35" s="4">
+        <v>23229</v>
+      </c>
+      <c r="G35" s="9">
+        <v>45</v>
+      </c>
+      <c r="H35" s="4">
+        <v>8554</v>
+      </c>
+      <c r="I35" s="6">
+        <v>103129</v>
+      </c>
+      <c r="J35" s="6">
+        <v>18100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="4">
+        <v>19456</v>
+      </c>
+      <c r="E36" s="4">
+        <v>18547</v>
+      </c>
+      <c r="G36" s="9">
+        <v>57</v>
+      </c>
+      <c r="H36" s="4">
+        <v>7165</v>
+      </c>
+      <c r="I36" s="6">
+        <v>91809</v>
+      </c>
+      <c r="J36" s="6">
+        <v>19100</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="4">
+        <v>19241</v>
+      </c>
+      <c r="D37" s="9">
+        <v>278</v>
+      </c>
+      <c r="E37" s="4">
+        <v>18570</v>
+      </c>
+      <c r="F37" s="9">
+        <v>421</v>
+      </c>
+      <c r="H37" s="4">
+        <v>7734</v>
+      </c>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="4">
+        <v>18491</v>
+      </c>
+      <c r="D38" s="9">
+        <v>179</v>
+      </c>
+      <c r="E38" s="4">
+        <v>21417</v>
+      </c>
+      <c r="F38" s="9">
+        <v>638</v>
+      </c>
+      <c r="H38" s="4">
+        <v>6577</v>
+      </c>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="4">
+        <v>19607</v>
+      </c>
+      <c r="E39" s="4">
+        <v>23935</v>
+      </c>
+      <c r="G39" s="9">
+        <v>58</v>
+      </c>
+      <c r="H39" s="4">
+        <v>6676</v>
+      </c>
+      <c r="I39" s="6">
+        <v>52431</v>
+      </c>
+      <c r="J39" s="6">
+        <v>13466</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="4">
+        <v>20827</v>
+      </c>
+      <c r="E40" s="4">
+        <v>20730</v>
+      </c>
+      <c r="G40" s="9">
         <v>50</v>
       </c>
-      <c r="B34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="4">
-        <v>21015</v>
-      </c>
-      <c r="E34" s="4">
-        <v>22503</v>
-      </c>
-      <c r="G34" s="10">
-        <v>20</v>
-      </c>
-      <c r="H34" s="4">
-        <v>7269</v>
-      </c>
-      <c r="I34" s="6">
-        <v>23888</v>
-      </c>
-      <c r="J34" s="6">
-        <v>4317</v>
+      <c r="H40" s="4">
+        <v>6137</v>
+      </c>
+      <c r="I40" s="6">
+        <v>50446</v>
+      </c>
+      <c r="J40" s="6">
+        <v>13247</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="4">
-        <v>20035</v>
-      </c>
-      <c r="E35" s="4">
-        <v>21379</v>
-      </c>
-      <c r="G35" s="10">
-        <v>56</v>
-      </c>
-      <c r="H35" s="4">
-        <v>5610</v>
-      </c>
-      <c r="I35" s="6">
-        <v>21979</v>
-      </c>
-      <c r="J35" s="6">
-        <v>4592</v>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="4">
+        <v>16040</v>
+      </c>
+      <c r="D41" s="9">
+        <v>2529</v>
+      </c>
+      <c r="E41" s="4">
+        <v>22257</v>
+      </c>
+      <c r="F41" s="9">
+        <v>8586</v>
+      </c>
+      <c r="G41" s="9">
+        <v>136</v>
+      </c>
+      <c r="H41" s="4">
+        <v>7100</v>
+      </c>
+      <c r="I41" s="6">
+        <v>7721</v>
+      </c>
+      <c r="J41" s="6">
+        <v>1166</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="4">
+        <v>15055</v>
+      </c>
+      <c r="D42" s="9">
+        <v>143</v>
+      </c>
+      <c r="E42" s="4">
+        <v>18207</v>
+      </c>
+      <c r="F42" s="9">
+        <v>13898</v>
+      </c>
+      <c r="G42" s="9">
+        <v>145</v>
+      </c>
+      <c r="H42" s="4">
+        <v>4255</v>
+      </c>
+      <c r="I42" s="6">
+        <v>11574</v>
+      </c>
+      <c r="J42" s="6">
+        <v>1888</v>
+      </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="4">
-        <v>21318</v>
-      </c>
-      <c r="E37" s="4">
-        <v>22962</v>
-      </c>
-      <c r="G37" s="10">
-        <v>51</v>
-      </c>
-      <c r="H37" s="4">
-        <v>6649</v>
-      </c>
-      <c r="I37" s="6">
-        <v>10924</v>
-      </c>
-      <c r="J37" s="6">
-        <v>1984</v>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="4">
+        <v>16714</v>
+      </c>
+      <c r="D43" s="9">
+        <v>22148</v>
+      </c>
+      <c r="E43" s="4">
+        <v>18432</v>
+      </c>
+      <c r="F43" s="9">
+        <v>65058</v>
+      </c>
+      <c r="G43" s="9">
+        <v>41</v>
+      </c>
+      <c r="H43" s="4">
+        <v>7808</v>
+      </c>
+      <c r="I43" s="6">
+        <v>50315</v>
+      </c>
+      <c r="J43" s="6">
+        <v>7069</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="4">
-        <v>18656</v>
-      </c>
-      <c r="E38" s="4">
-        <v>22022</v>
-      </c>
-      <c r="G38" s="10">
-        <v>66</v>
-      </c>
-      <c r="H38" s="4">
-        <v>6151</v>
-      </c>
-      <c r="I38" s="6">
-        <v>10280</v>
-      </c>
-      <c r="J38" s="6">
-        <v>2340</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40" s="4">
-        <v>21217</v>
-      </c>
-      <c r="E40" s="4">
-        <v>22085</v>
-      </c>
-      <c r="G40" s="10">
-        <v>17</v>
-      </c>
-      <c r="H40" s="4">
-        <v>9374</v>
-      </c>
-      <c r="I40" s="6">
-        <v>17934</v>
-      </c>
-      <c r="J40" s="6">
-        <v>3190</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="4">
-        <v>17999</v>
-      </c>
-      <c r="E41" s="4">
-        <v>21987</v>
-      </c>
-      <c r="G41" s="10">
-        <v>74</v>
-      </c>
-      <c r="H41" s="4">
-        <v>6044</v>
-      </c>
-      <c r="I41" s="6">
-        <v>16816</v>
-      </c>
-      <c r="J41" s="6">
-        <v>3571</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C44" s="4">
-        <v>19278</v>
-      </c>
-      <c r="D44" s="10">
-        <v>593</v>
+        <v>21549</v>
+      </c>
+      <c r="D44" s="9">
+        <v>44075</v>
       </c>
       <c r="E44" s="4">
-        <v>20047</v>
-      </c>
-      <c r="F44" s="10">
-        <v>5142</v>
+        <v>18499</v>
+      </c>
+      <c r="F44" s="9">
+        <v>120149</v>
+      </c>
+      <c r="G44" s="9">
+        <v>1120</v>
       </c>
       <c r="H44" s="4">
-        <v>7847</v>
-      </c>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
-        <v>20</v>
-      </c>
-      <c r="C45" s="4">
-        <v>19311</v>
-      </c>
-      <c r="D45" s="10">
-        <v>559</v>
-      </c>
-      <c r="E45" s="4">
-        <v>20412</v>
-      </c>
-      <c r="F45" s="10">
-        <v>5383</v>
-      </c>
-      <c r="H45" s="4">
-        <v>6459</v>
-      </c>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="4">
-        <v>21519</v>
-      </c>
-      <c r="E46" s="4">
-        <v>23229</v>
-      </c>
-      <c r="G46" s="10">
-        <v>45</v>
-      </c>
-      <c r="H46" s="4">
-        <v>8554</v>
-      </c>
-      <c r="I46" s="6">
-        <v>103129</v>
-      </c>
-      <c r="J46" s="6">
-        <v>18100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
-        <v>24</v>
-      </c>
-      <c r="C47" s="4">
-        <v>19456</v>
-      </c>
-      <c r="E47" s="4">
-        <v>18547</v>
-      </c>
-      <c r="G47" s="10">
-        <v>57</v>
-      </c>
-      <c r="H47" s="4">
-        <v>7165</v>
-      </c>
-      <c r="I47" s="6">
-        <v>91809</v>
-      </c>
-      <c r="J47" s="6">
-        <v>19100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C48" s="4"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="1"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" s="4">
-        <v>19241</v>
-      </c>
-      <c r="D49" s="10">
-        <v>278</v>
-      </c>
-      <c r="E49" s="4">
-        <v>18570</v>
-      </c>
-      <c r="F49" s="10">
-        <v>421</v>
-      </c>
-      <c r="H49" s="4">
-        <v>7734</v>
-      </c>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B50" t="s">
-        <v>17</v>
-      </c>
-      <c r="C50" s="4">
-        <v>18491</v>
-      </c>
-      <c r="D50" s="10">
-        <v>179</v>
-      </c>
-      <c r="E50" s="4">
-        <v>21417</v>
-      </c>
-      <c r="F50" s="10">
-        <v>638</v>
-      </c>
-      <c r="H50" s="4">
-        <v>6577</v>
-      </c>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B51" t="s">
-        <v>26</v>
-      </c>
-      <c r="C51" s="4">
-        <v>19607</v>
-      </c>
-      <c r="E51" s="4">
-        <v>23935</v>
-      </c>
-      <c r="G51" s="10">
-        <v>58</v>
-      </c>
-      <c r="H51" s="4">
-        <v>6676</v>
-      </c>
-      <c r="I51" s="6">
-        <v>52431</v>
-      </c>
-      <c r="J51" s="6">
-        <v>13466</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B52" t="s">
-        <v>26</v>
-      </c>
-      <c r="C52" s="4">
-        <v>20827</v>
-      </c>
-      <c r="E52" s="4">
-        <v>20730</v>
-      </c>
-      <c r="G52" s="10">
-        <v>50</v>
-      </c>
-      <c r="H52" s="4">
-        <v>6137</v>
-      </c>
-      <c r="I52" s="6">
-        <v>50446</v>
-      </c>
-      <c r="J52" s="6">
-        <v>13247</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A55" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B56" t="s">
-        <v>27</v>
-      </c>
-      <c r="C56" s="4">
-        <v>16040</v>
-      </c>
-      <c r="D56" s="10">
-        <v>2529</v>
-      </c>
-      <c r="E56" s="4">
-        <v>22257</v>
-      </c>
-      <c r="F56" s="10">
-        <v>8586</v>
-      </c>
-      <c r="G56" s="10">
-        <v>136</v>
-      </c>
-      <c r="H56" s="4">
-        <v>7100</v>
-      </c>
-      <c r="I56" s="6">
-        <v>7721</v>
-      </c>
-      <c r="J56" s="6">
-        <v>1166</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B57" t="s">
-        <v>29</v>
-      </c>
-      <c r="C57" s="4">
-        <v>15055</v>
-      </c>
-      <c r="D57" s="10">
-        <v>143</v>
-      </c>
-      <c r="E57" s="4">
-        <v>18207</v>
-      </c>
-      <c r="F57" s="10">
-        <v>13898</v>
-      </c>
-      <c r="G57" s="10">
-        <v>145</v>
-      </c>
-      <c r="H57" s="4">
-        <v>4255</v>
-      </c>
-      <c r="I57" s="6">
-        <v>11574</v>
-      </c>
-      <c r="J57" s="6">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B58" t="s">
-        <v>28</v>
-      </c>
-      <c r="C58" s="4">
-        <v>16714</v>
-      </c>
-      <c r="D58" s="10">
-        <v>22148</v>
-      </c>
-      <c r="E58" s="4">
-        <v>18432</v>
-      </c>
-      <c r="F58" s="10">
-        <v>65058</v>
-      </c>
-      <c r="G58" s="10">
-        <v>41</v>
-      </c>
-      <c r="H58" s="4">
-        <v>7808</v>
-      </c>
-      <c r="I58" s="6">
-        <v>50315</v>
-      </c>
-      <c r="J58" s="6">
-        <v>7069</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B59" t="s">
-        <v>21</v>
-      </c>
-      <c r="C59" s="4">
-        <v>21549</v>
-      </c>
-      <c r="D59" s="10">
-        <v>44075</v>
-      </c>
-      <c r="E59" s="4">
-        <v>18499</v>
-      </c>
-      <c r="F59" s="10">
-        <v>120149</v>
-      </c>
-      <c r="G59" s="10">
-        <v>1120</v>
-      </c>
-      <c r="H59" s="4">
         <v>10755</v>
       </c>
-      <c r="I59" s="6">
+      <c r="I44" s="6">
         <v>99718</v>
       </c>
-      <c r="J59" s="6">
+      <c r="J44" s="6">
         <v>12557</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="C1:L99">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="C1:L84">
     <sortCondition ref="C4:L4"/>
   </sortState>
-  <mergeCells count="3">
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A55:H55"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>